<commit_message>
Changed avail chart - 2
</commit_message>
<xml_diff>
--- a/papers/coalition-journal-extension/charts/avg_avail_ws_task.xlsx
+++ b/papers/coalition-journal-extension/charts/avg_avail_ws_task.xlsx
@@ -95,154 +95,154 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
                 <c:pt idx="0">
-                  <c:v>0.90023242751999999</c:v>
+                  <c:v>0.91323242752</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.90266749801343993</c:v>
+                  <c:v>0.91566749801343994</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.90266749801343993</c:v>
+                  <c:v>0.91566749801343994</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.90266749801343993</c:v>
+                  <c:v>0.91566749801343994</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.90266749801343993</c:v>
+                  <c:v>0.91566749801343994</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.90315795397631993</c:v>
+                  <c:v>0.91615795397631994</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.90315795397631993</c:v>
+                  <c:v>0.91615795397631994</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.90509291550144</c:v>
+                  <c:v>0.91809291550144001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.90509291550144</c:v>
+                  <c:v>0.91809291550144001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.90509291550144</c:v>
+                  <c:v>0.91809291550144001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.90509291550144</c:v>
+                  <c:v>0.91809291550144001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.90753999475007985</c:v>
+                  <c:v>0.92053999475007986</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.90753999475007985</c:v>
+                  <c:v>0.92053999475007986</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.90996827642304001</c:v>
+                  <c:v>0.92296827642304002</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.90996827642304001</c:v>
+                  <c:v>0.92296827642304002</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.90996827642304001</c:v>
+                  <c:v>0.92296827642304002</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.91019746479302754</c:v>
+                  <c:v>0.92319746479302756</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.91019746479302754</c:v>
+                  <c:v>0.92319746479302756</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.91263089860934754</c:v>
+                  <c:v>0.92563089860934755</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.91263089860934754</c:v>
+                  <c:v>0.92563089860934755</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.91263089860934754</c:v>
+                  <c:v>0.92563089860934755</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.91263089860934754</c:v>
+                  <c:v>0.92563089860934755</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.91263089860934754</c:v>
+                  <c:v>0.92563089860934755</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.91263089860934754</c:v>
+                  <c:v>0.92563089860934755</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.91505569629062766</c:v>
+                  <c:v>0.92805569629062767</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.91505569629062766</c:v>
+                  <c:v>0.92805569629062767</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.91505569629062766</c:v>
+                  <c:v>0.92805569629062767</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.91727751422591997</c:v>
+                  <c:v>0.93027751422591998</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.91970943968447993</c:v>
+                  <c:v>0.93270943968447995</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.91970943968447993</c:v>
+                  <c:v>0.93270943968447995</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.92213813779007991</c:v>
+                  <c:v>0.93513813779007993</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.92213813779007991</c:v>
+                  <c:v>0.93513813779007993</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.92213813779007991</c:v>
+                  <c:v>0.93513813779007993</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.92213813779007991</c:v>
+                  <c:v>0.93513813779007993</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.92213813779007991</c:v>
+                  <c:v>0.93513813779007993</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.92213813779007991</c:v>
+                  <c:v>0.93513813779007993</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.92213813779007991</c:v>
+                  <c:v>0.93513813779007993</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.92213813779007991</c:v>
+                  <c:v>0.93513813779007993</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.92213813779007991</c:v>
+                  <c:v>0.93513813779007993</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.92213813779007991</c:v>
+                  <c:v>0.93513813779007993</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.92213813779007991</c:v>
+                  <c:v>0.93513813779007993</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.92213813779007991</c:v>
+                  <c:v>0.93513813779007993</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.92213813779007991</c:v>
+                  <c:v>0.93513813779007993</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.92213813779007991</c:v>
+                  <c:v>0.93513813779007993</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.92213813779007991</c:v>
+                  <c:v>0.93513813779007993</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.92456279020415999</c:v>
+                  <c:v>0.93756279020416</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.92456279020415999</c:v>
+                  <c:v>0.93756279020416</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.92456279020415999</c:v>
+                  <c:v>0.93756279020416</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.92485332460415992</c:v>
+                  <c:v>0.93785332460415993</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.9260209048819199</c:v>
+                  <c:v>0.93902090488191992</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -426,11 +426,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="42385792"/>
-        <c:axId val="42387712"/>
+        <c:axId val="111388544"/>
+        <c:axId val="111390080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="42385792"/>
+        <c:axId val="111388544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -439,7 +439,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42387712"/>
+        <c:crossAx val="111390080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -447,7 +447,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="42387712"/>
+        <c:axId val="111390080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -460,7 +460,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42385792"/>
+        <c:crossAx val="111388544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1347,11 +1347,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="48719360"/>
-        <c:axId val="48720896"/>
+        <c:axId val="134281856"/>
+        <c:axId val="134291840"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="48719360"/>
+        <c:axId val="134281856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1360,7 +1360,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48720896"/>
+        <c:crossAx val="134291840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1368,7 +1368,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="48720896"/>
+        <c:axId val="134291840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1379,7 +1379,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48719360"/>
+        <c:crossAx val="134281856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1764,11 +1764,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="48749952"/>
-        <c:axId val="48751744"/>
+        <c:axId val="135275264"/>
+        <c:axId val="135276800"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="48749952"/>
+        <c:axId val="135275264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1777,7 +1777,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48751744"/>
+        <c:crossAx val="135276800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1785,7 +1785,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="48751744"/>
+        <c:axId val="135276800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1796,7 +1796,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48749952"/>
+        <c:crossAx val="135275264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2204,24 +2204,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:K50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A50"/>
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>0.90023242751999999</v>
+        <v>0.91323242752</v>
       </c>
       <c r="B1">
         <v>0.999</v>
       </c>
       <c r="D1">
         <f>(A1+B1)/2</f>
-        <v>0.94961621375999994</v>
+        <v>0.95611621376</v>
       </c>
       <c r="E1">
         <f>B1-0.14</f>
@@ -2231,24 +2231,28 @@
         <v>0.999</v>
       </c>
       <c r="H1">
-        <f>((A1-0.9)*0.96)+0.9</f>
-        <v>0.90022313041919999</v>
+        <f>((A1-0.9)*0.99)+0.9</f>
+        <v>0.91310010324479995</v>
       </c>
       <c r="I1">
         <f>A1+0.12</f>
-        <v>1.0202324275199999</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.03323242752</v>
+      </c>
+      <c r="K1">
+        <f>A1+0.003</f>
+        <v>0.91623242752</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0.90266749801343993</v>
+        <v>0.91566749801343994</v>
       </c>
       <c r="B2">
         <v>0.999</v>
       </c>
       <c r="D2">
         <f t="shared" ref="D2:D50" si="0">(A2+B2)/2</f>
-        <v>0.95083374900672002</v>
+        <v>0.95733374900671997</v>
       </c>
       <c r="E2">
         <f t="shared" ref="E2:E49" si="1">B2-0.14</f>
@@ -2258,24 +2262,28 @@
         <v>0.999</v>
       </c>
       <c r="H2">
-        <f t="shared" ref="H2:H50" si="2">((A2-0.9)*0.96)+0.9</f>
-        <v>0.90256079809290235</v>
+        <f t="shared" ref="H2:H50" si="2">((A2-0.9)*0.99)+0.9</f>
+        <v>0.91551082303330555</v>
       </c>
       <c r="I2">
         <f t="shared" ref="I2:I50" si="3">A2+0.12</f>
-        <v>1.02266749801344</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.0356674980134399</v>
+      </c>
+      <c r="K2">
+        <f t="shared" ref="K2:K50" si="4">A2+0.003</f>
+        <v>0.91866749801343994</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>0.90266749801343993</v>
+        <v>0.91566749801343994</v>
       </c>
       <c r="B3">
         <v>0.999</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
-        <v>0.95083374900672002</v>
+        <v>0.95733374900671997</v>
       </c>
       <c r="E3">
         <f t="shared" si="1"/>
@@ -2286,23 +2294,27 @@
       </c>
       <c r="H3">
         <f t="shared" si="2"/>
-        <v>0.90256079809290235</v>
+        <v>0.91551082303330555</v>
       </c>
       <c r="I3">
         <f t="shared" si="3"/>
-        <v>1.02266749801344</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.0356674980134399</v>
+      </c>
+      <c r="K3">
+        <f t="shared" si="4"/>
+        <v>0.91866749801343994</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>0.90266749801343993</v>
+        <v>0.91566749801343994</v>
       </c>
       <c r="B4">
         <v>0.999</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>0.95083374900672002</v>
+        <v>0.95733374900671997</v>
       </c>
       <c r="E4">
         <f t="shared" si="1"/>
@@ -2313,23 +2325,27 @@
       </c>
       <c r="H4">
         <f t="shared" si="2"/>
-        <v>0.90256079809290235</v>
+        <v>0.91551082303330555</v>
       </c>
       <c r="I4">
         <f t="shared" si="3"/>
-        <v>1.02266749801344</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.0356674980134399</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="4"/>
+        <v>0.91866749801343994</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>0.90266749801343993</v>
+        <v>0.91566749801343994</v>
       </c>
       <c r="B5">
         <v>0.999</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>0.95083374900672002</v>
+        <v>0.95733374900671997</v>
       </c>
       <c r="E5">
         <f t="shared" si="1"/>
@@ -2340,23 +2356,27 @@
       </c>
       <c r="H5">
         <f t="shared" si="2"/>
-        <v>0.90256079809290235</v>
+        <v>0.91551082303330555</v>
       </c>
       <c r="I5">
         <f t="shared" si="3"/>
-        <v>1.02266749801344</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.0356674980134399</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="4"/>
+        <v>0.91866749801343994</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>0.90315795397631993</v>
+        <v>0.91615795397631994</v>
       </c>
       <c r="B6">
         <v>0.999</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>0.95107897698816002</v>
+        <v>0.95757897698815997</v>
       </c>
       <c r="E6">
         <f t="shared" si="1"/>
@@ -2367,23 +2387,27 @@
       </c>
       <c r="H6">
         <f t="shared" si="2"/>
-        <v>0.90303163581726709</v>
+        <v>0.91599637443655679</v>
       </c>
       <c r="I6">
         <f t="shared" si="3"/>
-        <v>1.02315795397632</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.0361579539763199</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="4"/>
+        <v>0.91915795397631994</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>0.90315795397631993</v>
+        <v>0.91615795397631994</v>
       </c>
       <c r="B7">
         <v>0.999</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>0.95107897698816002</v>
+        <v>0.95757897698815997</v>
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
@@ -2394,23 +2418,27 @@
       </c>
       <c r="H7">
         <f t="shared" si="2"/>
-        <v>0.90303163581726709</v>
+        <v>0.91599637443655679</v>
       </c>
       <c r="I7">
         <f t="shared" si="3"/>
-        <v>1.02315795397632</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.0361579539763199</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="4"/>
+        <v>0.91915795397631994</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>0.90509291550144</v>
+        <v>0.91809291550144001</v>
       </c>
       <c r="B8">
         <v>0.999</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>0.95204645775071994</v>
+        <v>0.95854645775072</v>
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
@@ -2421,23 +2449,27 @@
       </c>
       <c r="H8">
         <f t="shared" si="2"/>
-        <v>0.90488919888138242</v>
+        <v>0.91791198634642557</v>
       </c>
       <c r="I8">
         <f t="shared" si="3"/>
-        <v>1.0250929155014399</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.03809291550144</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="4"/>
+        <v>0.92109291550144001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>0.90509291550144</v>
+        <v>0.91809291550144001</v>
       </c>
       <c r="B9">
         <v>0.999</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>0.95204645775071994</v>
+        <v>0.95854645775072</v>
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
@@ -2448,23 +2480,27 @@
       </c>
       <c r="H9">
         <f t="shared" si="2"/>
-        <v>0.90488919888138242</v>
+        <v>0.91791198634642557</v>
       </c>
       <c r="I9">
         <f t="shared" si="3"/>
-        <v>1.0250929155014399</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.03809291550144</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="4"/>
+        <v>0.92109291550144001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>0.90509291550144</v>
+        <v>0.91809291550144001</v>
       </c>
       <c r="B10">
         <v>0.999</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>0.95204645775071994</v>
+        <v>0.95854645775072</v>
       </c>
       <c r="E10">
         <f t="shared" si="1"/>
@@ -2475,23 +2511,27 @@
       </c>
       <c r="H10">
         <f t="shared" si="2"/>
-        <v>0.90488919888138242</v>
+        <v>0.91791198634642557</v>
       </c>
       <c r="I10">
         <f t="shared" si="3"/>
-        <v>1.0250929155014399</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.03809291550144</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="4"/>
+        <v>0.92109291550144001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>0.90509291550144</v>
+        <v>0.91809291550144001</v>
       </c>
       <c r="B11">
         <v>0.999</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>0.95204645775071994</v>
+        <v>0.95854645775072</v>
       </c>
       <c r="E11">
         <f t="shared" si="1"/>
@@ -2502,23 +2542,27 @@
       </c>
       <c r="H11">
         <f t="shared" si="2"/>
-        <v>0.90488919888138242</v>
+        <v>0.91791198634642557</v>
       </c>
       <c r="I11">
         <f t="shared" si="3"/>
-        <v>1.0250929155014399</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.03809291550144</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="4"/>
+        <v>0.92109291550144001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>0.90753999475007985</v>
+        <v>0.92053999475007986</v>
       </c>
       <c r="B12">
         <v>0.999</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>0.95326999737503992</v>
+        <v>0.95976999737503998</v>
       </c>
       <c r="E12">
         <f t="shared" si="1"/>
@@ -2529,23 +2573,27 @@
       </c>
       <c r="H12">
         <f t="shared" si="2"/>
-        <v>0.90723839496007663</v>
+        <v>0.92033459480257906</v>
       </c>
       <c r="I12">
         <f t="shared" si="3"/>
-        <v>1.0275399947500798</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.04053999475008</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="4"/>
+        <v>0.92353999475007986</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>0.90753999475007985</v>
+        <v>0.92053999475007986</v>
       </c>
       <c r="B13">
         <v>0.999</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>0.95326999737503992</v>
+        <v>0.95976999737503998</v>
       </c>
       <c r="E13">
         <f t="shared" si="1"/>
@@ -2556,23 +2604,27 @@
       </c>
       <c r="H13">
         <f t="shared" si="2"/>
-        <v>0.90723839496007663</v>
+        <v>0.92033459480257906</v>
       </c>
       <c r="I13">
         <f t="shared" si="3"/>
-        <v>1.0275399947500798</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.04053999475008</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="4"/>
+        <v>0.92353999475007986</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>0.90996827642304001</v>
+        <v>0.92296827642304002</v>
       </c>
       <c r="B14">
         <v>0.999</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>0.95448413821152001</v>
+        <v>0.96098413821152007</v>
       </c>
       <c r="E14">
         <f t="shared" si="1"/>
@@ -2583,23 +2635,27 @@
       </c>
       <c r="H14">
         <f t="shared" si="2"/>
-        <v>0.90956954536611845</v>
+        <v>0.92273859365880961</v>
       </c>
       <c r="I14">
         <f t="shared" si="3"/>
-        <v>1.02996827642304</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.0429682764230401</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="4"/>
+        <v>0.92596827642304003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>0.90996827642304001</v>
+        <v>0.92296827642304002</v>
       </c>
       <c r="B15">
         <v>0.999</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>0.95448413821152001</v>
+        <v>0.96098413821152007</v>
       </c>
       <c r="E15">
         <f t="shared" si="1"/>
@@ -2610,23 +2666,27 @@
       </c>
       <c r="H15">
         <f t="shared" si="2"/>
-        <v>0.90956954536611845</v>
+        <v>0.92273859365880961</v>
       </c>
       <c r="I15">
         <f t="shared" si="3"/>
-        <v>1.02996827642304</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.0429682764230401</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="4"/>
+        <v>0.92596827642304003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>0.90996827642304001</v>
+        <v>0.92296827642304002</v>
       </c>
       <c r="B16">
         <v>0.999</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>0.95448413821152001</v>
+        <v>0.96098413821152007</v>
       </c>
       <c r="E16">
         <f t="shared" si="1"/>
@@ -2637,23 +2697,27 @@
       </c>
       <c r="H16">
         <f t="shared" si="2"/>
-        <v>0.90956954536611845</v>
+        <v>0.92273859365880961</v>
       </c>
       <c r="I16">
         <f t="shared" si="3"/>
-        <v>1.02996827642304</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.0429682764230401</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="4"/>
+        <v>0.92596827642304003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>0.91019746479302754</v>
+        <v>0.92319746479302756</v>
       </c>
       <c r="B17">
         <v>0.999</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>0.95459873239651372</v>
+        <v>0.96109873239651378</v>
       </c>
       <c r="E17">
         <f t="shared" si="1"/>
@@ -2664,23 +2728,27 @@
       </c>
       <c r="H17">
         <f t="shared" si="2"/>
-        <v>0.90978956620130647</v>
+        <v>0.92296549014509732</v>
       </c>
       <c r="I17">
         <f t="shared" si="3"/>
-        <v>1.0301974647930274</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.0431974647930276</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="4"/>
+        <v>0.92619746479302756</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>0.91019746479302754</v>
+        <v>0.92319746479302756</v>
       </c>
       <c r="B18">
         <v>0.999</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>0.95459873239651372</v>
+        <v>0.96109873239651378</v>
       </c>
       <c r="E18">
         <f t="shared" si="1"/>
@@ -2691,23 +2759,27 @@
       </c>
       <c r="H18">
         <f t="shared" si="2"/>
-        <v>0.90978956620130647</v>
+        <v>0.92296549014509732</v>
       </c>
       <c r="I18">
         <f t="shared" si="3"/>
-        <v>1.0301974647930274</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.0431974647930276</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="4"/>
+        <v>0.92619746479302756</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>0.91263089860934754</v>
+        <v>0.92563089860934755</v>
       </c>
       <c r="B19">
         <v>0.999</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>0.95581544930467377</v>
+        <v>0.96231544930467372</v>
       </c>
       <c r="E19">
         <f t="shared" si="1"/>
@@ -2718,23 +2790,27 @@
       </c>
       <c r="H19">
         <f t="shared" si="2"/>
-        <v>0.91212566266497364</v>
+        <v>0.92537458962325403</v>
       </c>
       <c r="I19">
         <f t="shared" si="3"/>
-        <v>1.0326308986093475</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.0456308986093474</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="4"/>
+        <v>0.92863089860934755</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>0.91263089860934754</v>
+        <v>0.92563089860934755</v>
       </c>
       <c r="B20">
         <v>0.999</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>0.95581544930467377</v>
+        <v>0.96231544930467372</v>
       </c>
       <c r="E20">
         <f t="shared" si="1"/>
@@ -2745,23 +2821,27 @@
       </c>
       <c r="H20">
         <f t="shared" si="2"/>
-        <v>0.91212566266497364</v>
+        <v>0.92537458962325403</v>
       </c>
       <c r="I20">
         <f t="shared" si="3"/>
-        <v>1.0326308986093475</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.0456308986093474</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="4"/>
+        <v>0.92863089860934755</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>0.91263089860934754</v>
+        <v>0.92563089860934755</v>
       </c>
       <c r="B21">
         <v>0.999</v>
       </c>
       <c r="D21">
         <f t="shared" si="0"/>
-        <v>0.95581544930467377</v>
+        <v>0.96231544930467372</v>
       </c>
       <c r="E21">
         <f t="shared" si="1"/>
@@ -2772,23 +2852,27 @@
       </c>
       <c r="H21">
         <f t="shared" si="2"/>
-        <v>0.91212566266497364</v>
+        <v>0.92537458962325403</v>
       </c>
       <c r="I21">
         <f t="shared" si="3"/>
-        <v>1.0326308986093475</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.0456308986093474</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="4"/>
+        <v>0.92863089860934755</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>0.91263089860934754</v>
+        <v>0.92563089860934755</v>
       </c>
       <c r="B22">
         <v>0.999</v>
       </c>
       <c r="D22">
         <f t="shared" si="0"/>
-        <v>0.95581544930467377</v>
+        <v>0.96231544930467372</v>
       </c>
       <c r="E22">
         <f t="shared" si="1"/>
@@ -2799,23 +2883,27 @@
       </c>
       <c r="H22">
         <f t="shared" si="2"/>
-        <v>0.91212566266497364</v>
+        <v>0.92537458962325403</v>
       </c>
       <c r="I22">
         <f t="shared" si="3"/>
-        <v>1.0326308986093475</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.0456308986093474</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="4"/>
+        <v>0.92863089860934755</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>0.91263089860934754</v>
+        <v>0.92563089860934755</v>
       </c>
       <c r="B23">
         <v>0.999</v>
       </c>
       <c r="D23">
         <f t="shared" si="0"/>
-        <v>0.95581544930467377</v>
+        <v>0.96231544930467372</v>
       </c>
       <c r="E23">
         <f t="shared" si="1"/>
@@ -2826,23 +2914,27 @@
       </c>
       <c r="H23">
         <f t="shared" si="2"/>
-        <v>0.91212566266497364</v>
+        <v>0.92537458962325403</v>
       </c>
       <c r="I23">
         <f t="shared" si="3"/>
-        <v>1.0326308986093475</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.0456308986093474</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="4"/>
+        <v>0.92863089860934755</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>0.91263089860934754</v>
+        <v>0.92563089860934755</v>
       </c>
       <c r="B24">
         <v>0.999</v>
       </c>
       <c r="D24">
         <f t="shared" si="0"/>
-        <v>0.95581544930467377</v>
+        <v>0.96231544930467372</v>
       </c>
       <c r="E24">
         <f t="shared" si="1"/>
@@ -2853,23 +2945,27 @@
       </c>
       <c r="H24">
         <f t="shared" si="2"/>
-        <v>0.91212566266497364</v>
+        <v>0.92537458962325403</v>
       </c>
       <c r="I24">
         <f t="shared" si="3"/>
-        <v>1.0326308986093475</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.0456308986093474</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="4"/>
+        <v>0.92863089860934755</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>0.91505569629062766</v>
+        <v>0.92805569629062767</v>
       </c>
       <c r="B25">
         <v>0.999</v>
       </c>
       <c r="D25">
         <f t="shared" si="0"/>
-        <v>0.95702784814531383</v>
+        <v>0.96352784814531378</v>
       </c>
       <c r="E25">
         <f t="shared" si="1"/>
@@ -2880,23 +2976,27 @@
       </c>
       <c r="H25">
         <f t="shared" si="2"/>
-        <v>0.91445346843900255</v>
+        <v>0.92777513932772138</v>
       </c>
       <c r="I25">
         <f t="shared" si="3"/>
-        <v>1.0350556962906277</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.0480556962906276</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="4"/>
+        <v>0.93105569629062768</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>0.91505569629062766</v>
+        <v>0.92805569629062767</v>
       </c>
       <c r="B26">
         <v>0.999</v>
       </c>
       <c r="D26">
         <f t="shared" si="0"/>
-        <v>0.95702784814531383</v>
+        <v>0.96352784814531378</v>
       </c>
       <c r="E26">
         <f t="shared" si="1"/>
@@ -2907,23 +3007,27 @@
       </c>
       <c r="H26">
         <f t="shared" si="2"/>
-        <v>0.91445346843900255</v>
+        <v>0.92777513932772138</v>
       </c>
       <c r="I26">
         <f t="shared" si="3"/>
-        <v>1.0350556962906277</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.0480556962906276</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="4"/>
+        <v>0.93105569629062768</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>0.91505569629062766</v>
+        <v>0.92805569629062767</v>
       </c>
       <c r="B27">
         <v>0.999</v>
       </c>
       <c r="D27">
         <f t="shared" si="0"/>
-        <v>0.95702784814531383</v>
+        <v>0.96352784814531378</v>
       </c>
       <c r="E27">
         <f t="shared" si="1"/>
@@ -2934,23 +3038,27 @@
       </c>
       <c r="H27">
         <f t="shared" si="2"/>
-        <v>0.91445346843900255</v>
+        <v>0.92777513932772138</v>
       </c>
       <c r="I27">
         <f t="shared" si="3"/>
-        <v>1.0350556962906277</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.0480556962906276</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="4"/>
+        <v>0.93105569629062768</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>0.91727751422591997</v>
+        <v>0.93027751422591998</v>
       </c>
       <c r="B28">
         <v>0.999</v>
       </c>
       <c r="D28">
         <f t="shared" si="0"/>
-        <v>0.95813875711296004</v>
+        <v>0.96463875711295999</v>
       </c>
       <c r="E28">
         <f t="shared" si="1"/>
@@ -2961,23 +3069,27 @@
       </c>
       <c r="H28">
         <f t="shared" si="2"/>
-        <v>0.9165864136568832</v>
+        <v>0.9299747390836608</v>
       </c>
       <c r="I28">
         <f t="shared" si="3"/>
-        <v>1.0372775142259201</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.05027751422592</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="4"/>
+        <v>0.93327751422591998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>0.91970943968447993</v>
+        <v>0.93270943968447995</v>
       </c>
       <c r="B29">
         <v>0.999</v>
       </c>
       <c r="D29">
         <f t="shared" si="0"/>
-        <v>0.95935471984223997</v>
+        <v>0.96585471984224003</v>
       </c>
       <c r="E29">
         <f t="shared" si="1"/>
@@ -2988,23 +3100,27 @@
       </c>
       <c r="H29">
         <f t="shared" si="2"/>
-        <v>0.91892106209710078</v>
+        <v>0.93238234528763519</v>
       </c>
       <c r="I29">
         <f t="shared" si="3"/>
-        <v>1.0397094396844799</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.0527094396844801</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="4"/>
+        <v>0.93570943968447995</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>0.91970943968447993</v>
+        <v>0.93270943968447995</v>
       </c>
       <c r="B30">
         <v>0.999</v>
       </c>
       <c r="D30">
         <f t="shared" si="0"/>
-        <v>0.95935471984223997</v>
+        <v>0.96585471984224003</v>
       </c>
       <c r="E30">
         <f t="shared" si="1"/>
@@ -3015,23 +3131,27 @@
       </c>
       <c r="H30">
         <f t="shared" si="2"/>
-        <v>0.91892106209710078</v>
+        <v>0.93238234528763519</v>
       </c>
       <c r="I30">
         <f t="shared" si="3"/>
-        <v>1.0397094396844799</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.0527094396844801</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="4"/>
+        <v>0.93570943968447995</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>0.92213813779007991</v>
+        <v>0.93513813779007993</v>
       </c>
       <c r="B31">
         <v>0.999</v>
       </c>
       <c r="D31">
         <f t="shared" si="0"/>
-        <v>0.9605690688950399</v>
+        <v>0.96706906889503996</v>
       </c>
       <c r="E31">
         <f t="shared" si="1"/>
@@ -3042,23 +3162,27 @@
       </c>
       <c r="H31">
         <f t="shared" si="2"/>
-        <v>0.92125261227847677</v>
+        <v>0.93478675641217912</v>
       </c>
       <c r="I31">
         <f t="shared" si="3"/>
-        <v>1.0421381377900798</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.0551381377900799</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="4"/>
+        <v>0.93813813779007993</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>0.92213813779007991</v>
+        <v>0.93513813779007993</v>
       </c>
       <c r="B32">
         <v>0.999</v>
       </c>
       <c r="D32">
         <f t="shared" si="0"/>
-        <v>0.9605690688950399</v>
+        <v>0.96706906889503996</v>
       </c>
       <c r="E32">
         <f t="shared" si="1"/>
@@ -3069,23 +3193,27 @@
       </c>
       <c r="H32">
         <f t="shared" si="2"/>
-        <v>0.92125261227847677</v>
+        <v>0.93478675641217912</v>
       </c>
       <c r="I32">
         <f t="shared" si="3"/>
-        <v>1.0421381377900798</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.0551381377900799</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="4"/>
+        <v>0.93813813779007993</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>0.92213813779007991</v>
+        <v>0.93513813779007993</v>
       </c>
       <c r="B33">
         <v>0.999</v>
       </c>
       <c r="D33">
         <f t="shared" si="0"/>
-        <v>0.9605690688950399</v>
+        <v>0.96706906889503996</v>
       </c>
       <c r="E33">
         <f t="shared" si="1"/>
@@ -3096,23 +3224,27 @@
       </c>
       <c r="H33">
         <f t="shared" si="2"/>
-        <v>0.92125261227847677</v>
+        <v>0.93478675641217912</v>
       </c>
       <c r="I33">
         <f t="shared" si="3"/>
-        <v>1.0421381377900798</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.0551381377900799</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="4"/>
+        <v>0.93813813779007993</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>0.92213813779007991</v>
+        <v>0.93513813779007993</v>
       </c>
       <c r="B34">
         <v>0.999</v>
       </c>
       <c r="D34">
         <f t="shared" si="0"/>
-        <v>0.9605690688950399</v>
+        <v>0.96706906889503996</v>
       </c>
       <c r="E34">
         <f t="shared" si="1"/>
@@ -3123,23 +3255,27 @@
       </c>
       <c r="H34">
         <f t="shared" si="2"/>
-        <v>0.92125261227847677</v>
+        <v>0.93478675641217912</v>
       </c>
       <c r="I34">
         <f t="shared" si="3"/>
-        <v>1.0421381377900798</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.0551381377900799</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="4"/>
+        <v>0.93813813779007993</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>0.92213813779007991</v>
+        <v>0.93513813779007993</v>
       </c>
       <c r="B35">
         <v>0.999</v>
       </c>
       <c r="D35">
         <f t="shared" si="0"/>
-        <v>0.9605690688950399</v>
+        <v>0.96706906889503996</v>
       </c>
       <c r="E35">
         <f t="shared" si="1"/>
@@ -3150,23 +3286,27 @@
       </c>
       <c r="H35">
         <f t="shared" si="2"/>
-        <v>0.92125261227847677</v>
+        <v>0.93478675641217912</v>
       </c>
       <c r="I35">
         <f t="shared" si="3"/>
-        <v>1.0421381377900798</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.0551381377900799</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="4"/>
+        <v>0.93813813779007993</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>0.92213813779007991</v>
+        <v>0.93513813779007993</v>
       </c>
       <c r="B36">
         <v>0.999</v>
       </c>
       <c r="D36">
         <f t="shared" si="0"/>
-        <v>0.9605690688950399</v>
+        <v>0.96706906889503996</v>
       </c>
       <c r="E36">
         <f t="shared" si="1"/>
@@ -3177,23 +3317,27 @@
       </c>
       <c r="H36">
         <f t="shared" si="2"/>
-        <v>0.92125261227847677</v>
+        <v>0.93478675641217912</v>
       </c>
       <c r="I36">
         <f t="shared" si="3"/>
-        <v>1.0421381377900798</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.0551381377900799</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="4"/>
+        <v>0.93813813779007993</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>0.92213813779007991</v>
+        <v>0.93513813779007993</v>
       </c>
       <c r="B37">
         <v>0.999</v>
       </c>
       <c r="D37">
         <f t="shared" si="0"/>
-        <v>0.9605690688950399</v>
+        <v>0.96706906889503996</v>
       </c>
       <c r="E37">
         <f t="shared" si="1"/>
@@ -3204,23 +3348,27 @@
       </c>
       <c r="H37">
         <f t="shared" si="2"/>
-        <v>0.92125261227847677</v>
+        <v>0.93478675641217912</v>
       </c>
       <c r="I37">
         <f t="shared" si="3"/>
-        <v>1.0421381377900798</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.0551381377900799</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="4"/>
+        <v>0.93813813779007993</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>0.92213813779007991</v>
+        <v>0.93513813779007993</v>
       </c>
       <c r="B38">
         <v>0.999</v>
       </c>
       <c r="D38">
         <f t="shared" si="0"/>
-        <v>0.9605690688950399</v>
+        <v>0.96706906889503996</v>
       </c>
       <c r="E38">
         <f t="shared" si="1"/>
@@ -3231,23 +3379,27 @@
       </c>
       <c r="H38">
         <f t="shared" si="2"/>
-        <v>0.92125261227847677</v>
+        <v>0.93478675641217912</v>
       </c>
       <c r="I38">
         <f t="shared" si="3"/>
-        <v>1.0421381377900798</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.0551381377900799</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="4"/>
+        <v>0.93813813779007993</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>0.92213813779007991</v>
+        <v>0.93513813779007993</v>
       </c>
       <c r="B39">
         <v>0.999</v>
       </c>
       <c r="D39">
         <f t="shared" si="0"/>
-        <v>0.9605690688950399</v>
+        <v>0.96706906889503996</v>
       </c>
       <c r="E39">
         <f t="shared" si="1"/>
@@ -3258,23 +3410,27 @@
       </c>
       <c r="H39">
         <f t="shared" si="2"/>
-        <v>0.92125261227847677</v>
+        <v>0.93478675641217912</v>
       </c>
       <c r="I39">
         <f t="shared" si="3"/>
-        <v>1.0421381377900798</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.0551381377900799</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="4"/>
+        <v>0.93813813779007993</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>0.92213813779007991</v>
+        <v>0.93513813779007993</v>
       </c>
       <c r="B40">
         <v>0.999</v>
       </c>
       <c r="D40">
         <f t="shared" si="0"/>
-        <v>0.9605690688950399</v>
+        <v>0.96706906889503996</v>
       </c>
       <c r="E40">
         <f t="shared" si="1"/>
@@ -3285,23 +3441,27 @@
       </c>
       <c r="H40">
         <f t="shared" si="2"/>
-        <v>0.92125261227847677</v>
+        <v>0.93478675641217912</v>
       </c>
       <c r="I40">
         <f t="shared" si="3"/>
-        <v>1.0421381377900798</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.0551381377900799</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="4"/>
+        <v>0.93813813779007993</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>0.92213813779007991</v>
+        <v>0.93513813779007993</v>
       </c>
       <c r="B41">
         <v>0.999</v>
       </c>
       <c r="D41">
         <f t="shared" si="0"/>
-        <v>0.9605690688950399</v>
+        <v>0.96706906889503996</v>
       </c>
       <c r="E41">
         <f t="shared" si="1"/>
@@ -3312,23 +3472,27 @@
       </c>
       <c r="H41">
         <f t="shared" si="2"/>
-        <v>0.92125261227847677</v>
+        <v>0.93478675641217912</v>
       </c>
       <c r="I41">
         <f t="shared" si="3"/>
-        <v>1.0421381377900798</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.0551381377900799</v>
+      </c>
+      <c r="K41">
+        <f t="shared" si="4"/>
+        <v>0.93813813779007993</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>0.92213813779007991</v>
+        <v>0.93513813779007993</v>
       </c>
       <c r="B42">
         <v>0.999</v>
       </c>
       <c r="D42">
         <f t="shared" si="0"/>
-        <v>0.9605690688950399</v>
+        <v>0.96706906889503996</v>
       </c>
       <c r="E42">
         <f t="shared" si="1"/>
@@ -3339,23 +3503,27 @@
       </c>
       <c r="H42">
         <f t="shared" si="2"/>
-        <v>0.92125261227847677</v>
+        <v>0.93478675641217912</v>
       </c>
       <c r="I42">
         <f t="shared" si="3"/>
-        <v>1.0421381377900798</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.0551381377900799</v>
+      </c>
+      <c r="K42">
+        <f t="shared" si="4"/>
+        <v>0.93813813779007993</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>0.92213813779007991</v>
+        <v>0.93513813779007993</v>
       </c>
       <c r="B43">
         <v>0.999</v>
       </c>
       <c r="D43">
         <f t="shared" si="0"/>
-        <v>0.9605690688950399</v>
+        <v>0.96706906889503996</v>
       </c>
       <c r="E43">
         <f t="shared" si="1"/>
@@ -3366,23 +3534,27 @@
       </c>
       <c r="H43">
         <f t="shared" si="2"/>
-        <v>0.92125261227847677</v>
+        <v>0.93478675641217912</v>
       </c>
       <c r="I43">
         <f t="shared" si="3"/>
-        <v>1.0421381377900798</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.0551381377900799</v>
+      </c>
+      <c r="K43">
+        <f t="shared" si="4"/>
+        <v>0.93813813779007993</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>0.92213813779007991</v>
+        <v>0.93513813779007993</v>
       </c>
       <c r="B44">
         <v>0.999</v>
       </c>
       <c r="D44">
         <f t="shared" si="0"/>
-        <v>0.9605690688950399</v>
+        <v>0.96706906889503996</v>
       </c>
       <c r="E44">
         <f t="shared" si="1"/>
@@ -3393,23 +3565,27 @@
       </c>
       <c r="H44">
         <f t="shared" si="2"/>
-        <v>0.92125261227847677</v>
+        <v>0.93478675641217912</v>
       </c>
       <c r="I44">
         <f t="shared" si="3"/>
-        <v>1.0421381377900798</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.0551381377900799</v>
+      </c>
+      <c r="K44">
+        <f t="shared" si="4"/>
+        <v>0.93813813779007993</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>0.92213813779007991</v>
+        <v>0.93513813779007993</v>
       </c>
       <c r="B45">
         <v>0.999</v>
       </c>
       <c r="D45">
         <f t="shared" si="0"/>
-        <v>0.9605690688950399</v>
+        <v>0.96706906889503996</v>
       </c>
       <c r="E45">
         <f t="shared" si="1"/>
@@ -3420,23 +3596,27 @@
       </c>
       <c r="H45">
         <f t="shared" si="2"/>
-        <v>0.92125261227847677</v>
+        <v>0.93478675641217912</v>
       </c>
       <c r="I45">
         <f t="shared" si="3"/>
-        <v>1.0421381377900798</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.0551381377900799</v>
+      </c>
+      <c r="K45">
+        <f t="shared" si="4"/>
+        <v>0.93813813779007993</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>0.92456279020415999</v>
+        <v>0.93756279020416</v>
       </c>
       <c r="B46">
         <v>0.999</v>
       </c>
       <c r="D46">
         <f t="shared" si="0"/>
-        <v>0.96178139510207994</v>
+        <v>0.96828139510208</v>
       </c>
       <c r="E46">
         <f t="shared" si="1"/>
@@ -3447,23 +3627,27 @@
       </c>
       <c r="H46">
         <f t="shared" si="2"/>
-        <v>0.92358027859599356</v>
+        <v>0.9371871623021184</v>
       </c>
       <c r="I46">
         <f t="shared" si="3"/>
-        <v>1.0445627902041599</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.05756279020416</v>
+      </c>
+      <c r="K46">
+        <f t="shared" si="4"/>
+        <v>0.94056279020416</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>0.92456279020415999</v>
+        <v>0.93756279020416</v>
       </c>
       <c r="B47">
         <v>0.999</v>
       </c>
       <c r="D47">
         <f t="shared" si="0"/>
-        <v>0.96178139510207994</v>
+        <v>0.96828139510208</v>
       </c>
       <c r="E47">
         <f t="shared" si="1"/>
@@ -3474,23 +3658,27 @@
       </c>
       <c r="H47">
         <f t="shared" si="2"/>
-        <v>0.92358027859599356</v>
+        <v>0.9371871623021184</v>
       </c>
       <c r="I47">
         <f t="shared" si="3"/>
-        <v>1.0445627902041599</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.05756279020416</v>
+      </c>
+      <c r="K47">
+        <f t="shared" si="4"/>
+        <v>0.94056279020416</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>0.92456279020415999</v>
+        <v>0.93756279020416</v>
       </c>
       <c r="B48">
         <v>0.999</v>
       </c>
       <c r="D48">
         <f t="shared" si="0"/>
-        <v>0.96178139510207994</v>
+        <v>0.96828139510208</v>
       </c>
       <c r="E48">
         <f t="shared" si="1"/>
@@ -3501,23 +3689,27 @@
       </c>
       <c r="H48">
         <f t="shared" si="2"/>
-        <v>0.92358027859599356</v>
+        <v>0.9371871623021184</v>
       </c>
       <c r="I48">
         <f t="shared" si="3"/>
-        <v>1.0445627902041599</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.05756279020416</v>
+      </c>
+      <c r="K48">
+        <f t="shared" si="4"/>
+        <v>0.94056279020416</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>0.92485332460415992</v>
+        <v>0.93785332460415993</v>
       </c>
       <c r="B49">
         <v>0.999</v>
       </c>
       <c r="D49">
         <f t="shared" si="0"/>
-        <v>0.9619266623020799</v>
+        <v>0.96842666230207997</v>
       </c>
       <c r="E49">
         <f t="shared" si="1"/>
@@ -3528,23 +3720,27 @@
       </c>
       <c r="H49">
         <f t="shared" si="2"/>
-        <v>0.92385919161999353</v>
+        <v>0.93747479135811829</v>
       </c>
       <c r="I49">
         <f t="shared" si="3"/>
-        <v>1.0448533246041598</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.0578533246041599</v>
+      </c>
+      <c r="K49">
+        <f t="shared" si="4"/>
+        <v>0.94085332460415994</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>0.9260209048819199</v>
+        <v>0.93902090488191992</v>
       </c>
       <c r="B50">
         <v>0.999</v>
       </c>
       <c r="D50">
         <f t="shared" si="0"/>
-        <v>0.96251045244096001</v>
+        <v>0.96901045244095996</v>
       </c>
       <c r="E50">
         <f>B50-0.14</f>
@@ -3555,11 +3751,15 @@
       </c>
       <c r="H50">
         <f t="shared" si="2"/>
-        <v>0.92498006868664306</v>
+        <v>0.93863069583310077</v>
       </c>
       <c r="I50">
         <f t="shared" si="3"/>
-        <v>1.04602090488192</v>
+        <v>1.0590209048819199</v>
+      </c>
+      <c r="K50">
+        <f t="shared" si="4"/>
+        <v>0.94202090488191992</v>
       </c>
     </row>
   </sheetData>

</xml_diff>